<commit_message>
Excel To DB working as intended - pyhton module
</commit_message>
<xml_diff>
--- a/Database/test DB.xlsx
+++ b/Database/test DB.xlsx
@@ -1,19 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Bath CW\IP20\Git\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Bath CW\IP20\Git\Database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6286C282-95F1-4F0E-96AD-2A6F558477CF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77ADA67A-F519-4E5F-B6FA-CDF3E23F28E4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="STYLE" sheetId="1" r:id="rId1"/>
+    <sheet name="AUTHOR" sheetId="2" r:id="rId2"/>
+    <sheet name="ART_PIECE" sheetId="3" r:id="rId3"/>
+    <sheet name="PLACE" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="47">
   <si>
     <t>Name</t>
   </si>
@@ -51,14 +54,884 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>DDDD</t>
+    <t>Style</t>
+  </si>
+  <si>
+    <t>Born</t>
+  </si>
+  <si>
+    <t>Death</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>city</t>
+  </si>
+  <si>
+    <t>Realism</t>
+  </si>
+  <si>
+    <t>This movement was a reaction against romanticism. Romanticism was an earlier movement that presented the world in much more idealized terms. </t>
+  </si>
+  <si>
+    <t>author</t>
+  </si>
+  <si>
+    <t>the angelus</t>
+  </si>
+  <si>
+    <t>1875 </t>
+  </si>
+  <si>
+    <t>Jean-François Millet</t>
+  </si>
+  <si>
+    <r>
+      <t> French painter and one of the founders of the </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FF0B0080"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Barbizon school</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> in rural France. Millet is noted for his scenes of peasant farmers; he can be categorized as part of the </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FF0B0080"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Realism art movement</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>The painting depicts two peasants bowing in a field over a basket of potatoes to say a prayer, the </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FF0B0080"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Angelus</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>, that together with the ringing of the bell from the church on the horizon marks the end of a day's work. Millet was commissioned by the American would-be painter and art collector Thomas Gold Appleton, who never came to collect it. The painting is famous today for driving the prices for artworks of the Barbizon school up to record amounts in the late 19th century.</t>
+    </r>
+  </si>
+  <si>
+    <t>Le Déjeuner sur l'herbe</t>
+  </si>
+  <si>
+    <t>Édouard Manet</t>
+  </si>
+  <si>
+    <t>1883 </t>
+  </si>
+  <si>
+    <t>Pablo Picasso</t>
+  </si>
+  <si>
+    <r>
+      <t>Guernica</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="19.8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Georgia"/>
+        <family val="1"/>
+      </rPr>
+      <t> </t>
+    </r>
+  </si>
+  <si>
+    <t>Cubism</t>
+  </si>
+  <si>
+    <t>The Weeping Woman</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>Beaux Arts</t>
+  </si>
+  <si>
+    <t>United-Kingdom</t>
+  </si>
+  <si>
+    <t>Bath</t>
+  </si>
+  <si>
+    <t>price</t>
+  </si>
+  <si>
+    <t>Beaux Arts is the longest established commercial gallery in Bath and has been located in the same beautiful building for nearly forty years. Beaux Arts Bath is the sister gallery to Beaux Arts in Maddox Street, London W1S.</t>
+  </si>
+  <si>
+    <t>The Bath Gallery</t>
+  </si>
+  <si>
+    <t>None but it can't be empty so :(</t>
+  </si>
+  <si>
+    <t>The louvre</t>
+  </si>
+  <si>
+    <t>France</t>
+  </si>
+  <si>
+    <t>Paris</t>
+  </si>
+  <si>
+    <t>flemme de remplir mais le louvre tu connais</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Pablo Ruiz Picasso </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>was a Spanish painter, sculptor, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FF0B0080"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>printmaker</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FF0B0080"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>ceramicist</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FF0B0080"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>stage designer</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>, poet and playwright who spent most of his adult life in France. Regarded as one of the most influential artists of the 20th century, he is known for co-founding the </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FF0B0080"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Cubist</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> movement, the invention of </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FF0B0080"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>constructed sculpture</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>,the co-invention of </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FF0B0080"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>collage</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>, and for the wide variety of styles that he helped develop and explore. Among his most famous works are the </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FF0B0080"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>proto-Cubist</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="7"/>
+        <color rgb="FF0B0080"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Les Demoiselles d'Avignon</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> (1907), and </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="7"/>
+        <color rgb="FF0B0080"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Guernica</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> (1937), a dramatic portrayal of the </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FF0B0080"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>bombing of Guernica</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> by the German and Italian airforces during the </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FF0B0080"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Spanish Civil War</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Born into an upper-class household with strong political connections, Manet rejected the future originally envisioned for him, and became engrossed in the world of painting. His early masterworks, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="7"/>
+        <color rgb="FF0B0080"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>The Luncheon on the Grass (Le dejeuner sur l'herbe)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> and </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="7"/>
+        <color rgb="FF0B0080"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Olympia</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>, both 1863, caused great controversy and served as rallying points for the young painters who would create Impressionism. Today, these are considered watershed paintings that mark the start of </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FF0B0080"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>modern art</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>. The last 20 years of Manet's life saw him form bonds with other great artists of the time, and develop his own style that would be heralded as innovative and serve as a major influence for future painters.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Guernica </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>is a large 1937 oil painting on canvas by </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FF0B0080"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Spanish</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> artist </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="7"/>
+        <color rgb="FF0B0080"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Pablo Picasso</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>. One of Picasso's best known works, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="7"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Guernica</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> is regarded by many art critics as one of the most moving and powerful </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FF0B0080"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>anti-war</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> paintings in history, It is exhibited in the </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FF0B0080"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Museo Reina Sofia</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> in Madrid.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Le Déjeuner sur l'herbe</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="7"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>The Luncheon on the Grass</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>) originally titled </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="7"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Le Bain</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> (</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="7"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>The Bath</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>)  is a large </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FF0B0080"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>oil on canvas</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> painting by E</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FF0B0080"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>douard Manet</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> created in 1862 and 1863. It depicts a </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FF0B0080"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>female nude</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> and a scantily dressed female bather on a picnic with two fully dressed men in a rural setting. Rejected by the </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FF0B0080"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Salon</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> jury of 1863, Manet seized the opportunity to exhibit this and two other paintings in the 1863 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FF0B0080"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Salon des Refusés</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>, where the painting sparked public notoriety and controversy. The piece is now in the </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FF0B0080"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Musee d'Orsay</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> in </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FF0B0080"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Paris</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>. A smaller, earlier version can be seen at the </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FF0B0080"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Courtauld Gallery</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FF0B0080"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>London</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>The Weeping Woman</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> is an </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FF0B0080"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>oil on canvas</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> painted by </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FF0B0080"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Pablo Picasso</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> in France in 1937. Picasso was intrigued with the subject, and revisited the theme numerous times that year. This painting, created on 26 October 1937, was the most elaborate of the series. Its dimensions are 60 x 49 cm. It has been in the collection of the </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FF0B0080"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Tate Modern</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> in </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FF0B0080"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>London</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> since 1987, and is currently located there.</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -72,16 +945,130 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF222222"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="19.8"/>
+      <color rgb="FF000000"/>
+      <name val="Georgia"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="19.8"/>
+      <color rgb="FF000000"/>
+      <name val="Georgia"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="6"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color rgb="FF222222"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color rgb="FF0B0080"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="7"/>
+      <color rgb="FF222222"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="7"/>
+      <color rgb="FF222222"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="7"/>
+      <color rgb="FF0B0080"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="7"/>
+      <color rgb="FF222222"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="7"/>
+      <color rgb="FF0B0080"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="15"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF8F9FA"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -89,17 +1076,81 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFA2A9B1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFA2A9B1"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFA2A9B1"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFA2A9B1"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFA2A9B1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFA2A9B1"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFA2A9B1"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFA2A9B1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -380,8 +1431,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -407,7 +1458,7 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>219</v>
+        <v>18</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>4</v>
@@ -415,10 +1466,10 @@
     </row>
     <row r="3" spans="1:3" ht="50" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="B3">
-        <v>120</v>
+        <v>19</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>6</v>
@@ -426,12 +1477,14 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="B4">
-        <v>3494</v>
-      </c>
-      <c r="C4" s="1"/>
+        <v>19</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
@@ -442,4 +1495,297 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80551813-DF97-4B59-B110-47D1D9456295}">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="17.36328125" customWidth="1"/>
+    <col min="2" max="2" width="17.08984375" customWidth="1"/>
+    <col min="3" max="3" width="9.36328125" customWidth="1"/>
+    <col min="5" max="5" width="46.1796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="4">
+        <v>1814</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="4">
+        <v>1832</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="50.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="4">
+        <v>1881</v>
+      </c>
+      <c r="D4">
+        <v>1973</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>42</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A3" r:id="rId1" tooltip="Édouard Manet" display="https://en.wikipedia.org/wiki/%C3%89douard_Manet" xr:uid="{A34A5D84-F623-44F5-9DBF-9BD4DD80EF8A}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1B3563B-B2DC-41C9-9759-6ECC277B2C9D}">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="20.54296875" customWidth="1"/>
+    <col min="2" max="2" width="14" customWidth="1"/>
+    <col min="3" max="3" width="14.08984375" customWidth="1"/>
+    <col min="4" max="4" width="22" customWidth="1"/>
+    <col min="5" max="5" width="102.90625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="4">
+        <v>1859</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="11">
+        <v>1863</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="25.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="4">
+        <v>1937</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="75.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" s="4">
+        <v>1937</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>46</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B3" r:id="rId1" tooltip="Édouard Manet" display="https://en.wikipedia.org/wiki/%C3%89douard_Manet" xr:uid="{FE1606DE-E5F5-48E3-9B2E-9E90CB479811}"/>
+    <hyperlink ref="B4" r:id="rId2" display="https://en.wikipedia.org/wiki/Pablo_Picasso" xr:uid="{6A90CB75-D0DE-460F-BD9D-C548E592799F}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3EF6DB2-2FDE-4CEB-ABE4-610163CC9DE7}">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="22.08984375" customWidth="1"/>
+    <col min="2" max="2" width="19.36328125" customWidth="1"/>
+    <col min="3" max="3" width="19.453125" customWidth="1"/>
+    <col min="4" max="4" width="14" customWidth="1"/>
+    <col min="5" max="5" width="15" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="19" x14ac:dyDescent="0.4">
+      <c r="A2" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" s="16" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="19" x14ac:dyDescent="0.4">
+      <c r="A3" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4">
+        <v>15</v>
+      </c>
+      <c r="C4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>